<commit_message>
modifying the items and creating new Class
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>CocaCola</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>Pepsi</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Smokic</t>
   </si>
 </sst>
 </file>
@@ -850,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -902,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -914,6 +920,28 @@
       </c>
       <c r="C5">
         <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>12313</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>11111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>